<commit_message>
graphs coefficient plots. uses same Conditions for everything via.
</commit_message>
<xml_diff>
--- a/res/LabDataNA.xlsx
+++ b/res/LabDataNA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2beccdac4dd3df76/DELL LAPTOP/Uni/RMIT/Tutoring/AERO2579 - Principles of Aerodynamics/Lab2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8950fd6461f21ca6/Documents/Assignments/Y2S1/PrincpAero/W4/data_calculator/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="11_18C293CA179C82440FD48A4116832444A10895E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F2C899A-32BB-45B5-A413-DFEFBC8C5986}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_18C293CA179C82440FD48A4116832444A10895E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{022F9182-6906-452D-89A0-2C65788BC107}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VDAS Data" sheetId="1" r:id="rId1"/>
@@ -253,32 +253,6 @@
     <t>(mbar)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Segoe UI"/>
-      </rPr>
-      <t>(kg.m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Segoe UI"/>
-      </rPr>
-      <t>-3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Segoe UI"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>(mm)</t>
   </si>
   <si>
@@ -331,6 +305,28 @@
   </si>
   <si>
     <t>Data Series 17</t>
+  </si>
+  <si>
+    <r>
+      <t>(kg.m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Segoe UI"/>
+      </rPr>
+      <t>-3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Segoe UI"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -478,13 +474,13 @@
     <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -928,93 +924,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AP8" sqref="AP8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="16.5" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="14.59765625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.86328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="20.265625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9.3984375" style="7" customWidth="1"/>
     <col min="7" max="7" width="13" style="5" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="10" customWidth="1"/>
-    <col min="9" max="38" width="9.140625" style="11" customWidth="1"/>
-    <col min="39" max="39" width="9.140625" style="12" customWidth="1"/>
-    <col min="40" max="40" width="26.28515625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" style="10" customWidth="1"/>
+    <col min="9" max="38" width="9.1328125" style="11" customWidth="1"/>
+    <col min="39" max="39" width="9.1328125" style="12" customWidth="1"/>
+    <col min="40" max="40" width="26.265625" style="8" customWidth="1"/>
     <col min="41" max="41" width="22" style="4" customWidth="1"/>
-    <col min="42" max="42" width="20.42578125" style="5" customWidth="1"/>
-    <col min="43" max="43" width="14.28515625" style="8" customWidth="1"/>
-    <col min="44" max="44" width="22.5703125" style="9" customWidth="1"/>
-    <col min="45" max="45" width="9.140625" style="1" customWidth="1"/>
-    <col min="46" max="16384" width="9.140625" style="1"/>
+    <col min="42" max="42" width="20.3984375" style="5" customWidth="1"/>
+    <col min="43" max="43" width="14.265625" style="8" customWidth="1"/>
+    <col min="44" max="44" width="22.59765625" style="9" customWidth="1"/>
+    <col min="45" max="45" width="9.1328125" style="1" customWidth="1"/>
+    <col min="46" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="18" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="20"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="16"/>
       <c r="AN1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="16"/>
+      <c r="AO1" s="18"/>
+      <c r="AP1" s="19"/>
       <c r="AQ1" s="21" t="s">
         <v>6</v>
       </c>
       <c r="AR1" s="22"/>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1036,40 +1032,40 @@
       <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="19"/>
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="20"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15"/>
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="15"/>
+      <c r="AM2" s="16"/>
       <c r="AN2" s="8" t="s">
         <v>14</v>
       </c>
@@ -1086,7 +1082,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.6">
       <c r="H3" s="10" t="s">
         <v>19</v>
       </c>
@@ -1184,7 +1180,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:44" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" ht="17.25" x14ac:dyDescent="0.6">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -1309,21 +1305,21 @@
         <v>59</v>
       </c>
       <c r="AP4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AQ4" s="8" t="s">
+      <c r="AR4" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="AR4" s="9" t="s">
-        <v>61</v>
-      </c>
     </row>
-    <row r="5" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -1457,7 +1453,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1591,7 +1587,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1725,7 +1721,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1859,7 +1855,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1993,12 +1989,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A11" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A12" s="2">
         <v>0</v>
       </c>
@@ -2132,7 +2128,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A13" s="2">
         <v>2</v>
       </c>
@@ -2266,7 +2262,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -2400,7 +2396,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A15" s="2">
         <v>6</v>
       </c>
@@ -2534,7 +2530,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:44" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:44" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A16" s="2">
         <v>8</v>
       </c>
@@ -2668,12 +2664,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A17" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A18" s="2">
         <v>0</v>
       </c>
@@ -2807,7 +2803,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -2941,7 +2937,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A20" s="2">
         <v>4</v>
       </c>
@@ -3075,7 +3071,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -3209,7 +3205,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:44" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:44" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A22" s="2">
         <v>8</v>
       </c>
@@ -3343,12 +3339,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A23" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A24" s="2">
         <v>0</v>
       </c>
@@ -3482,7 +3478,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A25" s="2">
         <v>2</v>
       </c>
@@ -3616,7 +3612,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A26" s="2">
         <v>4</v>
       </c>
@@ -3750,7 +3746,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A27" s="2">
         <v>6</v>
       </c>
@@ -3884,7 +3880,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:44" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:44" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A28" s="2">
         <v>8</v>
       </c>
@@ -4018,12 +4014,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A29" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A30" s="2">
         <v>0</v>
       </c>
@@ -4157,7 +4153,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A31" s="2">
         <v>2</v>
       </c>
@@ -4291,7 +4287,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A32" s="2">
         <v>4</v>
       </c>
@@ -4425,7 +4421,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A33" s="2">
         <v>6</v>
       </c>
@@ -4559,7 +4555,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A34" s="2">
         <v>8</v>
       </c>
@@ -4693,12 +4689,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A35" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A36" s="2">
         <v>0</v>
       </c>
@@ -4832,7 +4828,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A37" s="2">
         <v>2</v>
       </c>
@@ -4966,7 +4962,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A38" s="2">
         <v>4</v>
       </c>
@@ -5100,7 +5096,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A39" s="2">
         <v>6</v>
       </c>
@@ -5234,7 +5230,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A40" s="2">
         <v>8</v>
       </c>
@@ -5368,12 +5364,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A41" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A42" s="2">
         <v>0</v>
       </c>
@@ -5507,7 +5503,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A43" s="2">
         <v>2</v>
       </c>
@@ -5641,7 +5637,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A44" s="2">
         <v>4</v>
       </c>
@@ -5775,7 +5771,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A45" s="2">
         <v>6</v>
       </c>
@@ -5909,7 +5905,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A46" s="2">
         <v>8</v>
       </c>
@@ -6043,12 +6039,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="47" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A47" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A48" s="2">
         <v>0</v>
       </c>
@@ -6182,7 +6178,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A49" s="2">
         <v>2</v>
       </c>
@@ -6316,7 +6312,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A50" s="2">
         <v>4</v>
       </c>
@@ -6450,7 +6446,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A51" s="2">
         <v>6</v>
       </c>
@@ -6584,7 +6580,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A52" s="2">
         <v>8</v>
       </c>
@@ -6718,12 +6714,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A53" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A54" s="2">
         <v>0</v>
       </c>
@@ -6857,7 +6853,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A55" s="2">
         <v>2</v>
       </c>
@@ -6991,7 +6987,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A56" s="2">
         <v>4</v>
       </c>
@@ -7125,7 +7121,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A57" s="2">
         <v>6</v>
       </c>
@@ -7259,7 +7255,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A58" s="2">
         <v>8</v>
       </c>
@@ -7393,12 +7389,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A59" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A60" s="2">
         <v>0</v>
       </c>
@@ -7532,7 +7528,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A61" s="2">
         <v>2</v>
       </c>
@@ -7666,7 +7662,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A62" s="2">
         <v>4</v>
       </c>
@@ -7800,7 +7796,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="63" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A63" s="2">
         <v>6</v>
       </c>
@@ -7934,7 +7930,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="64" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A64" s="2">
         <v>8</v>
       </c>
@@ -8068,12 +8064,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="65" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A65" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A66" s="2">
         <v>0</v>
       </c>
@@ -8207,7 +8203,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A67" s="2">
         <v>2</v>
       </c>
@@ -8341,7 +8337,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A68" s="2">
         <v>4</v>
       </c>
@@ -8475,7 +8471,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A69" s="2">
         <v>6</v>
       </c>
@@ -8609,7 +8605,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="70" spans="1:44" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:44" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A70" s="2">
         <v>8</v>
       </c>
@@ -8743,12 +8739,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A71" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A72" s="2">
         <v>0</v>
       </c>
@@ -8882,7 +8878,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A73" s="2">
         <v>2</v>
       </c>
@@ -9016,7 +9012,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A74" s="2">
         <v>4</v>
       </c>
@@ -9150,7 +9146,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A75" s="2">
         <v>6</v>
       </c>
@@ -9284,7 +9280,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="76" spans="1:44" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:44" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A76" s="2">
         <v>8</v>
       </c>
@@ -9418,12 +9414,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A77" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A78" s="2">
         <v>0</v>
       </c>
@@ -9557,7 +9553,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A79" s="2">
         <v>2</v>
       </c>
@@ -9691,7 +9687,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A80" s="2">
         <v>4</v>
       </c>
@@ -9825,7 +9821,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="81" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A81" s="2">
         <v>6</v>
       </c>
@@ -9959,7 +9955,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="82" spans="1:44" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:44" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A82" s="2">
         <v>8</v>
       </c>
@@ -10093,12 +10089,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A83" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A84" s="2">
         <v>0</v>
       </c>
@@ -10232,7 +10228,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A85" s="2">
         <v>2</v>
       </c>
@@ -10366,7 +10362,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="86" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A86" s="2">
         <v>4</v>
       </c>
@@ -10500,7 +10496,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A87" s="2">
         <v>6</v>
       </c>
@@ -10634,7 +10630,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="88" spans="1:44" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:44" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A88" s="2">
         <v>8</v>
       </c>
@@ -10768,12 +10764,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="89" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A89" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A90" s="2">
         <v>0</v>
       </c>
@@ -10907,7 +10903,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A91" s="2">
         <v>2</v>
       </c>
@@ -11041,7 +11037,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="92" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A92" s="2">
         <v>4</v>
       </c>
@@ -11175,7 +11171,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="93" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A93" s="2">
         <v>6</v>
       </c>
@@ -11309,7 +11305,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="94" spans="1:44" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:44" ht="16.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A94" s="2">
         <v>8</v>
       </c>
@@ -11443,12 +11439,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="95" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A95" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A96" s="2">
         <v>0</v>
       </c>
@@ -11582,7 +11578,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="97" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A97" s="2">
         <v>2</v>
       </c>
@@ -11716,7 +11712,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="98" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A98" s="2">
         <v>4</v>
       </c>
@@ -11850,7 +11846,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A99" s="2">
         <v>6</v>
       </c>
@@ -11984,7 +11980,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="100" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A100" s="2">
         <v>8</v>
       </c>
@@ -12118,12 +12114,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:44" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A101" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="102" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A102" s="2">
         <v>0</v>
       </c>
@@ -12257,7 +12253,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="103" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A103" s="2">
         <v>2</v>
       </c>
@@ -12391,7 +12387,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="104" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A104" s="2">
         <v>4</v>
       </c>
@@ -12525,7 +12521,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="105" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A105" s="2">
         <v>6</v>
       </c>
@@ -12659,7 +12655,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="106" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:44" x14ac:dyDescent="0.6">
       <c r="A106" s="2">
         <v>8</v>
       </c>
@@ -12795,12 +12791,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="H2:AM2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:AM1"/>
     <mergeCell ref="AN1:AP1"/>
-    <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:AR10">
     <cfRule type="expression" dxfId="17" priority="2">

</xml_diff>